<commit_message>
refactoring + example test case
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UiPath Projects\PopularUnicornNames\PopularUnicornNames\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F008666B-F6DE-44DE-AE48-8D36C59295B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{146391FB-3DC3-42A6-BD4A-296966DD89C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -582,15 +582,15 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="18.75">
+    <row r="1" spans="1:26" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -635,7 +635,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" s="2" t="s">
         <v>35</v>
       </c>
@@ -649,7 +649,7 @@
     <row r="4" spans="1:26">
       <c r="A4" s="2"/>
     </row>
-    <row r="5" spans="1:26" ht="30">
+    <row r="5" spans="1:26" ht="28.8">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -732,15 +732,15 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="18.75">
+    <row r="1" spans="1:26" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -774,7 +774,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -785,7 +785,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -898,7 +898,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="28.8">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -923,12 +923,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>